<commit_message>
Aggiornati i file excel
Aggiunto valori e aggiornato i grafici
</commit_message>
<xml_diff>
--- a/first assignment/result_kruskal_naive.xlsx
+++ b/first assignment/result_kruskal_naive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davide/Sviluppo/Advanced Algorithm/first assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Desktop\Advanced Algorithm\AdvancedAlgorithms-assignments\first assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7966B2-D85B-354A-8C30-D9503C9AE0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E1A12B-22CE-481F-BEE1-67D770FBEDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="760" windowWidth="29140" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result_kruskal_naive" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>file</t>
   </si>
@@ -257,6 +257,21 @@
   </si>
   <si>
     <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>m*n</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>choosen const</t>
+  </si>
+  <si>
+    <t>Media I</t>
+  </si>
+  <si>
+    <t>m*n*const</t>
   </si>
 </sst>
 </file>
@@ -816,6 +831,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>KRUSKAL</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> NAIVE</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -855,7 +900,7 @@
           <c:x val="9.7437544395242354E-2"/>
           <c:y val="0.12060175404903657"/>
           <c:w val="0.86286955733220483"/>
-          <c:h val="0.80398361180462197"/>
+          <c:h val="0.71939902090187302"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -865,15 +910,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>result_kruskal_naive!$I$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Time (ms)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Measured Time (ms)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -901,7 +938,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>result_kruskal_naive!$H$8:$H$24</c:f>
+              <c:f>result_kruskal_naive!$U$2:$U$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -961,7 +998,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>result_kruskal_naive!$I$8:$I$24</c:f>
+              <c:f>result_kruskal_naive!$V$2:$V$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1023,6 +1060,163 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F378-E840-A40B-BD21293E216E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>0,00018*m*n</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>result_kruskal_naive!$J$2:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>result_kruskal_naive!$K$2:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.9350000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.1800000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37440000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.403</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.195999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>152.85599999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>237.82500000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>961.38000000000011</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3848.9399999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15405.84</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23957.550000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>96152.400000000009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>384159.60000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1536073.2000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2401182</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F805-4413-AA14-505204E2694C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1059,6 +1253,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Number of vertices</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1104,6 +1353,7 @@
         <c:axId val="434630704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2700000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1122,6 +1372,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1171,6 +1476,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1768,16 +2104,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>100240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>740472</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133699</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2102,19 +2438,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2130,8 +2468,32 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2147,8 +2509,37 @@
       <c r="E2">
         <v>6.73</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <f>C2*B2</f>
+        <v>90</v>
+      </c>
+      <c r="G2">
+        <f>E2/F2</f>
+        <v>7.4777777777777776E-2</v>
+      </c>
+      <c r="H2">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I2">
+        <f>F2*H2</f>
+        <v>1.6200000000000003E-2</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGEIF(B:B,J2,I:I)</f>
+        <v>1.9350000000000003E-2</v>
+      </c>
+      <c r="U2">
+        <v>10</v>
+      </c>
+      <c r="V2">
+        <f>AVERAGEIF(B:B,U2,E:E)</f>
+        <v>1.7324999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2164,8 +2555,37 @@
       <c r="E3">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">C3*B3</f>
+        <v>110</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="1">E3/F3</f>
+        <v>7.2727272727272734E-4</v>
+      </c>
+      <c r="H3">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I66" si="2">F3*H3</f>
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <f>AVERAGEIF(B:B,J3,I:I)</f>
+        <v>9.1800000000000007E-2</v>
+      </c>
+      <c r="U3">
+        <v>20</v>
+      </c>
+      <c r="V3">
+        <f>AVERAGEIF(B:B,U3,E:E)</f>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2181,8 +2601,37 @@
       <c r="E4">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>4.6153846153846153E-4</v>
+      </c>
+      <c r="H4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>2.3400000000000001E-2</v>
+      </c>
+      <c r="J4">
+        <v>40</v>
+      </c>
+      <c r="K4">
+        <f>AVERAGEIF(B:B,J4,I:I)</f>
+        <v>0.37440000000000007</v>
+      </c>
+      <c r="U4">
+        <v>40</v>
+      </c>
+      <c r="V4">
+        <f>AVERAGEIF(B:B,U4,E:E)</f>
+        <v>0.34249999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2198,8 +2647,37 @@
       <c r="E5">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H5">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="J5">
+        <v>80</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGEIF(B:B,J5,I:I)</f>
+        <v>1.5300000000000002</v>
+      </c>
+      <c r="U5">
+        <v>80</v>
+      </c>
+      <c r="V5">
+        <f>AVERAGEIF(B:B,U5,E:E)</f>
+        <v>1.3225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2215,8 +2693,37 @@
       <c r="E6">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>2.7083333333333332E-4</v>
+      </c>
+      <c r="H6">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>8.6400000000000005E-2</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGEIF(B:B,J6,I:I)</f>
+        <v>2.403</v>
+      </c>
+      <c r="U6">
+        <v>100</v>
+      </c>
+      <c r="V6">
+        <f>AVERAGEIF(B:B,U6,E:E)</f>
+        <v>1.4375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2232,14 +2739,37 @@
       <c r="E7">
         <v>0.11</v>
       </c>
-      <c r="H7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>2.2916666666666666E-4</v>
+      </c>
+      <c r="H7">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>8.6400000000000005E-2</v>
+      </c>
+      <c r="J7">
+        <v>200</v>
+      </c>
+      <c r="K7">
+        <f>AVERAGEIF(B:B,J7,I:I)</f>
+        <v>9.6479999999999997</v>
+      </c>
+      <c r="U7">
+        <v>200</v>
+      </c>
+      <c r="V7">
+        <f>AVERAGEIF(B:B,U7,E:E)</f>
+        <v>6.9574999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2255,15 +2785,37 @@
       <c r="E8">
         <v>0.15</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>560</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>2.6785714285714287E-4</v>
+      </c>
       <c r="H8">
-        <v>10</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I8">
-        <f>AVERAGEIF(B:B,H8,E:E)</f>
-        <v>1.7324999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0.1008</v>
+      </c>
+      <c r="J8">
+        <v>400</v>
+      </c>
+      <c r="K8">
+        <f>AVERAGEIF(B:B,J8,I:I)</f>
+        <v>38.195999999999998</v>
+      </c>
+      <c r="U8">
+        <v>400</v>
+      </c>
+      <c r="V8">
+        <f>AVERAGEIF(B:B,U8,E:E)</f>
+        <v>19.022500000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2279,15 +2831,37 @@
       <c r="E9">
         <v>0.13</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>520</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
       <c r="H9">
-        <v>20</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9:I24" si="0">AVERAGEIF(B:B,H9,E:E)</f>
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>9.3600000000000003E-2</v>
+      </c>
+      <c r="J9">
+        <v>800</v>
+      </c>
+      <c r="K9">
+        <f>AVERAGEIF(B:B,J9,I:I)</f>
+        <v>152.85599999999999</v>
+      </c>
+      <c r="U9">
+        <v>800</v>
+      </c>
+      <c r="V9">
+        <f>AVERAGEIF(B:B,U9,E:E)</f>
+        <v>65.099999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2303,15 +2877,37 @@
       <c r="E10">
         <v>0.32</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2240</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1.4285714285714287E-4</v>
+      </c>
       <c r="H10">
-        <v>40</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
-        <v>0.34249999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0.4032</v>
+      </c>
+      <c r="J10">
+        <v>1000</v>
+      </c>
+      <c r="K10">
+        <f>AVERAGEIF(B:B,J10,I:I)</f>
+        <v>237.82500000000005</v>
+      </c>
+      <c r="U10">
+        <v>1000</v>
+      </c>
+      <c r="V10">
+        <f>AVERAGEIF(B:B,U10,E:E)</f>
+        <v>104.75999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2327,15 +2923,37 @@
       <c r="E11">
         <v>0.31</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>1.55E-4</v>
+      </c>
       <c r="H11">
-        <v>80</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
-        <v>1.3225</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0.36000000000000004</v>
+      </c>
+      <c r="J11">
+        <v>2000</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGEIF(B:B,J11,I:I)</f>
+        <v>961.38000000000011</v>
+      </c>
+      <c r="U11">
+        <v>2000</v>
+      </c>
+      <c r="V11">
+        <f>AVERAGEIF(B:B,U11,E:E)</f>
+        <v>560.70000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2351,15 +2969,37 @@
       <c r="E12">
         <v>0.32</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>1.6000000000000001E-4</v>
+      </c>
       <c r="H12">
-        <v>100</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
-        <v>1.4375</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0.36000000000000004</v>
+      </c>
+      <c r="J12">
+        <v>4000</v>
+      </c>
+      <c r="K12">
+        <f>AVERAGEIF(B:B,J12,I:I)</f>
+        <v>3848.9399999999996</v>
+      </c>
+      <c r="U12">
+        <v>4000</v>
+      </c>
+      <c r="V12">
+        <f>AVERAGEIF(B:B,U12,E:E)</f>
+        <v>1709.1625000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2375,15 +3015,37 @@
       <c r="E13">
         <v>0.42</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>2080</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>2.0192307692307691E-4</v>
+      </c>
       <c r="H13">
-        <v>200</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
-        <v>6.9574999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>0.37440000000000001</v>
+      </c>
+      <c r="J13">
+        <v>8000</v>
+      </c>
+      <c r="K13">
+        <f>AVERAGEIF(B:B,J13,I:I)</f>
+        <v>15405.84</v>
+      </c>
+      <c r="U13">
+        <v>8000</v>
+      </c>
+      <c r="V13">
+        <f>AVERAGEIF(B:B,U13,E:E)</f>
+        <v>8083.12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2399,15 +3061,37 @@
       <c r="E14">
         <v>0.92</v>
       </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>8640</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>1.0648148148148149E-4</v>
+      </c>
       <c r="H14">
-        <v>400</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
-        <v>19.022500000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>1.5552000000000001</v>
+      </c>
+      <c r="J14">
+        <v>10000</v>
+      </c>
+      <c r="K14">
+        <f>AVERAGEIF(B:B,J14,I:I)</f>
+        <v>23957.550000000003</v>
+      </c>
+      <c r="U14">
+        <v>10000</v>
+      </c>
+      <c r="V14">
+        <f>AVERAGEIF(B:B,U14,E:E)</f>
+        <v>13780.455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2423,15 +3107,37 @@
       <c r="E15">
         <v>0.75</v>
       </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>7920</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>9.4696969696969697E-5</v>
+      </c>
       <c r="H15">
-        <v>800</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
-        <v>65.099999999999994</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>1.4256000000000002</v>
+      </c>
+      <c r="J15">
+        <v>20000</v>
+      </c>
+      <c r="K15">
+        <f>AVERAGEIF(B:B,J15,I:I)</f>
+        <v>96152.400000000009</v>
+      </c>
+      <c r="U15">
+        <v>20000</v>
+      </c>
+      <c r="V15">
+        <f>AVERAGEIF(B:B,U15,E:E)</f>
+        <v>63388.920000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2447,15 +3153,37 @@
       <c r="E16">
         <v>0.87</v>
       </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>8320</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1.0456730769230769E-4</v>
+      </c>
       <c r="H16">
-        <v>1000</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
-        <v>104.75999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>1.4976</v>
+      </c>
+      <c r="J16">
+        <v>40000</v>
+      </c>
+      <c r="K16">
+        <f>AVERAGEIF(B:B,J16,I:I)</f>
+        <v>384159.60000000003</v>
+      </c>
+      <c r="U16">
+        <v>40000</v>
+      </c>
+      <c r="V16">
+        <f>AVERAGEIF(B:B,U16,E:E)</f>
+        <v>314910.17749999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2471,15 +3199,37 @@
       <c r="E17">
         <v>2.75</v>
       </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>9120</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>3.0153508771929826E-4</v>
+      </c>
       <c r="H17">
-        <v>2000</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
-        <v>560.70000000000005</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>1.6416000000000002</v>
+      </c>
+      <c r="J17">
+        <v>80000</v>
+      </c>
+      <c r="K17">
+        <f>AVERAGEIF(B:B,J17,I:I)</f>
+        <v>1536073.2000000002</v>
+      </c>
+      <c r="U17">
+        <v>80000</v>
+      </c>
+      <c r="V17">
+        <f>AVERAGEIF(B:B,U17,E:E)</f>
+        <v>1556325.23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2495,15 +3245,37 @@
       <c r="E18">
         <v>1.53</v>
       </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>13600</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>1.125E-4</v>
+      </c>
       <c r="H18">
-        <v>4000</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I18">
-        <f t="shared" si="0"/>
-        <v>1709.1625000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>2.448</v>
+      </c>
+      <c r="J18">
+        <v>100000</v>
+      </c>
+      <c r="K18">
+        <f>AVERAGEIF(B:B,J18,I:I)</f>
+        <v>2401182</v>
+      </c>
+      <c r="U18">
+        <v>100000</v>
+      </c>
+      <c r="V18">
+        <f>AVERAGEIF(B:B,U18,E:E)</f>
+        <v>2504591.06</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2519,15 +3291,23 @@
       <c r="E19">
         <v>1.32</v>
       </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>12900</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>1.0232558139534884E-4</v>
+      </c>
       <c r="H19">
-        <v>8000</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
-        <v>8083.12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>2.3220000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2543,15 +3323,23 @@
       <c r="E20">
         <v>1.56</v>
       </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>13700</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>1.1386861313868613E-4</v>
+      </c>
       <c r="H20">
-        <v>10000</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
-        <v>13780.455</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>2.4660000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2567,15 +3355,23 @@
       <c r="E21">
         <v>1.34</v>
       </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>13200</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>1.0151515151515152E-4</v>
+      </c>
       <c r="H21">
-        <v>20000</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
-        <v>63388.920000000006</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>2.3760000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2591,15 +3387,23 @@
       <c r="E22">
         <v>4.58</v>
       </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>53400</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>8.5767790262172291E-5</v>
+      </c>
       <c r="H22">
-        <v>40000</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
-        <v>314910.17749999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>9.6120000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2615,15 +3419,23 @@
       <c r="E23">
         <v>5.42</v>
       </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>53800</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1.0074349442379182E-4</v>
+      </c>
       <c r="H23">
-        <v>80000</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I23">
-        <f t="shared" si="0"/>
-        <v>1556325.23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>9.6840000000000011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -2639,15 +3451,23 @@
       <c r="E24">
         <v>11.58</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>53800</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>2.1524163568773235E-4</v>
+      </c>
       <c r="H24">
-        <v>100000</v>
+        <v>1.8000000000000001E-4</v>
       </c>
       <c r="I24">
-        <f t="shared" si="0"/>
-        <v>2504591.06</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>9.6840000000000011</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -2663,8 +3483,23 @@
       <c r="E25">
         <v>6.25</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>53400</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>1.1704119850187266E-4</v>
+      </c>
+      <c r="H25">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>9.6120000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2680,8 +3515,23 @@
       <c r="E26">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>216000</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>9.3518518518518522E-5</v>
+      </c>
+      <c r="H26">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>38.880000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2697,8 +3547,23 @@
       <c r="E27">
         <v>18.21</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>207200</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>8.7886100386100384E-5</v>
+      </c>
+      <c r="H27">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>37.295999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -2714,8 +3579,23 @@
       <c r="E28">
         <v>16.46</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>215200</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>7.6486988847583649E-5</v>
+      </c>
+      <c r="H28">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>38.736000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -2731,8 +3611,23 @@
       <c r="E29">
         <v>21.22</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>210400</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1.0085551330798479E-4</v>
+      </c>
+      <c r="H29">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>37.872</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -2748,8 +3643,23 @@
       <c r="E30">
         <v>64.48</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>850400</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>7.5823142050799626E-5</v>
+      </c>
+      <c r="H30">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>153.072</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2765,8 +3675,23 @@
       <c r="E31">
         <v>66.59</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>846400</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>7.8674385633270325E-5</v>
+      </c>
+      <c r="H31">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>152.352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -2782,8 +3707,23 @@
       <c r="E32">
         <v>66.25</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>860800</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>7.6963289962825277E-5</v>
+      </c>
+      <c r="H32">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>154.94400000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2799,8 +3739,23 @@
       <c r="E33">
         <v>63.08</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>839200</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>7.5166825548141083E-5</v>
+      </c>
+      <c r="H33">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>151.05600000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2816,8 +3771,23 @@
       <c r="E34">
         <v>102.96</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>1300000</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>7.9200000000000001E-5</v>
+      </c>
+      <c r="H34">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>234.00000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2833,8 +3803,23 @@
       <c r="E35">
         <v>103.71</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>1313000</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>7.8987052551408979E-5</v>
+      </c>
+      <c r="H35">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>236.34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -2850,8 +3835,23 @@
       <c r="E36">
         <v>98.28</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>1328000</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>7.4006024096385541E-5</v>
+      </c>
+      <c r="H36">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>239.04000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -2867,8 +3867,23 @@
       <c r="E37">
         <v>114.09</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>1344000</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>8.4888392857142858E-5</v>
+      </c>
+      <c r="H37">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>241.92000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2884,8 +3899,23 @@
       <c r="E38">
         <v>567.25</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>5398000</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>1.0508521674694331E-4</v>
+      </c>
+      <c r="H38">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>971.6400000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -2901,8 +3931,23 @@
       <c r="E39">
         <v>529.51</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>5308000</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>9.9756970610399398E-5</v>
+      </c>
+      <c r="H39">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>955.44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -2918,8 +3963,23 @@
       <c r="E40">
         <v>545.35</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>5304000</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>1.0281862745098039E-4</v>
+      </c>
+      <c r="H40">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>954.72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -2935,8 +3995,23 @@
       <c r="E41">
         <v>600.69000000000005</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>5354000</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>1.1219462084422862E-4</v>
+      </c>
+      <c r="H41">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>963.72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -2952,8 +4027,23 @@
       <c r="E42" s="1">
         <v>2151.79</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>21440000</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>1.003633395522388E-4</v>
+      </c>
+      <c r="H42">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="2"/>
+        <v>3859.2000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -2969,8 +4059,23 @@
       <c r="E43" s="1">
         <v>1841.63</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>21260000</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>8.66241768579492E-5</v>
+      </c>
+      <c r="H43">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="2"/>
+        <v>3826.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -2986,8 +4091,23 @@
       <c r="E44" s="1">
         <v>1407.26</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>21360000</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>6.5882958801498121E-5</v>
+      </c>
+      <c r="H44">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>3844.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -3003,8 +4123,23 @@
       <c r="E45" s="1">
         <v>1435.97</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>21472000</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>6.687639716840537E-5</v>
+      </c>
+      <c r="H45">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="2"/>
+        <v>3864.96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -3020,8 +4155,23 @@
       <c r="E46" s="1">
         <v>8198.43</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>85640000</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>9.573131714152266E-5</v>
+      </c>
+      <c r="H46">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="2"/>
+        <v>15415.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -3037,8 +4187,23 @@
       <c r="E47" s="1">
         <v>7316.72</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>85360000</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>8.5716026241799441E-5</v>
+      </c>
+      <c r="H47">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="2"/>
+        <v>15364.800000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -3054,8 +4219,23 @@
       <c r="E48" s="1">
         <v>8270.8799999999992</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>85296000</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>9.6966797974113659E-5</v>
+      </c>
+      <c r="H48">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="2"/>
+        <v>15353.28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -3071,8 +4251,23 @@
       <c r="E49" s="1">
         <v>8546.4500000000007</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>86056000</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>9.9312656874593294E-5</v>
+      </c>
+      <c r="H49">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="2"/>
+        <v>15490.080000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -3088,8 +4283,23 @@
       <c r="E50" s="1">
         <v>15195.1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>133010000</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="1"/>
+        <v>1.1424028268551237E-4</v>
+      </c>
+      <c r="H50">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="2"/>
+        <v>23941.800000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -3105,8 +4315,23 @@
       <c r="E51" s="1">
         <v>12725.11</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>133400000</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>9.539062968515743E-5</v>
+      </c>
+      <c r="H51">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="2"/>
+        <v>24012</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -3122,8 +4347,23 @@
       <c r="E52" s="1">
         <v>13479.76</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>132870000</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="1"/>
+        <v>1.0145074132610823E-4</v>
+      </c>
+      <c r="H52">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="2"/>
+        <v>23916.600000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -3139,8 +4379,23 @@
       <c r="E53" s="1">
         <v>13721.85</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>133110000</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>1.0308654496281272E-4</v>
+      </c>
+      <c r="H53">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="2"/>
+        <v>23959.800000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -3156,8 +4411,23 @@
       <c r="E54" s="1">
         <v>63173.72</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>533340000</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="1"/>
+        <v>1.1844924438444519E-4</v>
+      </c>
+      <c r="H54">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="2"/>
+        <v>96001.200000000012</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -3173,8 +4443,23 @@
       <c r="E55" s="1">
         <v>62115.73</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>536520000</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="1"/>
+        <v>1.1577523671065385E-4</v>
+      </c>
+      <c r="H55">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="2"/>
+        <v>96573.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -3190,8 +4475,23 @@
       <c r="E56" s="1">
         <v>65332.19</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>533460000</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="1"/>
+        <v>1.2246876991714469E-4</v>
+      </c>
+      <c r="H56">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="2"/>
+        <v>96022.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -3207,8 +4507,23 @@
       <c r="E57" s="1">
         <v>62934.04</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>533400000</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="1"/>
+        <v>1.1798657667791526E-4</v>
+      </c>
+      <c r="H57">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="2"/>
+        <v>96012</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -3224,8 +4539,23 @@
       <c r="E58" s="1">
         <v>398490.17</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>2136600000</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="1"/>
+        <v>1.8650667883553308E-4</v>
+      </c>
+      <c r="H58">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="2"/>
+        <v>384588</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -3241,8 +4571,23 @@
       <c r="E59" s="1">
         <v>299276.84000000003</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>2137840000</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="1"/>
+        <v>1.3999028926392997E-4</v>
+      </c>
+      <c r="H59">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="2"/>
+        <v>384811.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -3258,8 +4603,23 @@
       <c r="E60" s="1">
         <v>283955.7</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>2129680000</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="1"/>
+        <v>1.3333256639495137E-4</v>
+      </c>
+      <c r="H60">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="2"/>
+        <v>383342.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -3275,8 +4635,23 @@
       <c r="E61" s="1">
         <v>277918</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>2132760000</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="1"/>
+        <v>1.3030908306607401E-4</v>
+      </c>
+      <c r="H61">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="2"/>
+        <v>383896.80000000005</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -3292,8 +4667,23 @@
       <c r="E62" s="1">
         <v>1407901.94</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>8553120000</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>1.6460682651476887E-4</v>
+      </c>
+      <c r="H62">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="2"/>
+        <v>1539561.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -3309,8 +4699,23 @@
       <c r="E63" s="1">
         <v>1626809.48</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>8530640000</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="1"/>
+        <v>1.9070192623296727E-4</v>
+      </c>
+      <c r="H63">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="2"/>
+        <v>1535515.2000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -3326,8 +4731,23 @@
       <c r="E64" s="1">
         <v>1556122.31</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>8526880000</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="1"/>
+        <v>1.8249609587563096E-4</v>
+      </c>
+      <c r="H64">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="2"/>
+        <v>1534838.4000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -3343,8 +4763,23 @@
       <c r="E65" s="1">
         <v>1634467.19</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>8524320000</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="1"/>
+        <v>1.917416509469377E-4</v>
+      </c>
+      <c r="H65">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="2"/>
+        <v>1534377.6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -3360,8 +4795,23 @@
       <c r="E66" s="1">
         <v>2481919.08</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>13339500000</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="1"/>
+        <v>1.8605787923085574E-4</v>
+      </c>
+      <c r="H66">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="2"/>
+        <v>2401110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -3377,8 +4827,23 @@
       <c r="E67" s="1">
         <v>2420404.2599999998</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <f t="shared" ref="F67:F69" si="3">C67*B67</f>
+        <v>13321400000</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G69" si="4">E67/F67</f>
+        <v>1.8169293467653548E-4</v>
+      </c>
+      <c r="H67">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I67">
+        <f t="shared" ref="I67:I69" si="5">F67*H67</f>
+        <v>2397852</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -3394,8 +4859,23 @@
       <c r="E68" s="1">
         <v>2521292.7000000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>13352400000</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="4"/>
+        <v>1.8882692999011414E-4</v>
+      </c>
+      <c r="H68">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="5"/>
+        <v>2403432</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -3410,6 +4890,21 @@
       </c>
       <c r="E69" s="1">
         <v>2594748.2000000002</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="3"/>
+        <v>13346300000</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="4"/>
+        <v>1.9441704442429739E-4</v>
+      </c>
+      <c r="H69">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="5"/>
+        <v>2402334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>